<commit_message>
sections headers bgs and layout
</commit_message>
<xml_diff>
--- a/data/lunar.xlsx
+++ b/data/lunar.xlsx
@@ -4,9 +4,11 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="home-section" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="admins" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="about-section" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="works-section" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="about-section" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="projects-section" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="collaborators-section" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="contact-section" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="admins" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,24 +16,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>textblock</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>some text</t>
-  </si>
-  <si>
-    <t>campaign1.png</t>
-  </si>
-  <si>
-    <t>http://someurl.com/</t>
+    <t>background</t>
+  </si>
+  <si>
+    <t>sometext example</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>Lunar Studio is an alliance between skilled artists, writers and thinkers, to develop and publish creative artifacts. /n The Studio is an imagined space, carved out of busy, pressuredlives. It is intended to incubate wonderful, strange ideas and turn them into items which can be shared with others. /n Our intention is to enable our own independent creative work,and to work with people we really enjoy. We undertake passion projects without commercial backing by producing, funding and publishing collaboratively. /n We don't cater to anyones' needs or desires but our own and each others' in the process of creating. The products which emerge are allowed to be uncompromising, decadent, and a pleasure to make.</t>
+  </si>
+  <si>
+    <t>id/order</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Frankie and the moon</t>
+  </si>
+  <si>
+    <t>Prints and Concept Art</t>
+  </si>
+  <si>
+    <t>Bone Cards</t>
+  </si>
+  <si>
+    <t>requires</t>
+  </si>
+  <si>
+    <t>collaborators</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
   </si>
 </sst>
 </file>
@@ -43,14 +72,18 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,6 +131,14 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -303,9 +344,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="19.29"/>
+    <col customWidth="1" min="3" max="3" width="16.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -315,26 +356,18 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -346,8 +379,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="60.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -360,8 +419,44 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="27.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -374,7 +469,57 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
collaborators + contanct bg + media
</commit_message>
<xml_diff>
--- a/data/lunar.xlsx
+++ b/data/lunar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>textblock</t>
   </si>
@@ -24,9 +24,6 @@
     <t>background</t>
   </si>
   <si>
-    <t>sometext example</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -51,10 +48,41 @@
     <t>Bone Cards</t>
   </si>
   <si>
-    <t>requires</t>
-  </si>
-  <si>
-    <t>collaborators</t>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>Frank Lunar</t>
+  </si>
+  <si>
+    <t>Frank has over 12 years experience as a designer, specialising in illustration. He works from home in Observatory, Cape Town, where daily tasks include, but are not limited to children book illustrations, comic book illustrations, story boards, concept art and graphic design..</t>
+  </si>
+  <si>
+    <t>Zoë Boshoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoë is a poet and writer. She is also a full-time organisational development specialist, dedicated to  helping very useful and talented people resource their own passions. Lunar Studio is a space in which she is able to use this skill set to resource creative work in which she is directly involved. </t>
+  </si>
+  <si>
+    <t>Emma Malikwa</t>
+  </si>
+  <si>
+    <t>Emma is a traditional healer, or sangoma, trained in multiple African healing disciplines.</t>
+  </si>
+  <si>
+    <t>Soulplay</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Soulplay is the magical domain of High quality, handmade, bespoke dolls made by the fabric artist Zoë Nepgen at her sewing studio in. Soulplay is our distributor for the Frankie Book Series. For more info visit </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>www.soulplay.co.za</t>
+    </r>
   </si>
   <si>
     <t>Contact Us</t>
@@ -64,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -82,6 +110,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,6 +137,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -355,11 +390,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -383,7 +415,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -394,13 +426,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -423,22 +455,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -458,16 +490,55 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B5"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -483,12 +554,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>